<commit_message>
Fixing Some Bug (KNN Algorithm still have different value)
</commit_message>
<xml_diff>
--- a/DATA SANGGAR KRISPI RENDI_.xlsx
+++ b/DATA SANGGAR KRISPI RENDI_.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\; DATA SKRIPSI\SEMPRO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\KNN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4EB6896-94F6-4095-8331-308BDCD0CB57}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8001013-C828-4FC8-A9BB-C5F18B15E9D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DATA" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="CONTOH STUDI KASUS" sheetId="3" r:id="rId3"/>
     <sheet name="Perhitungan Studi Kasus" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="88">
   <si>
     <t>Bulan Maret</t>
   </si>
@@ -328,6 +328,9 @@
   </si>
   <si>
     <t>ED (2,4,2)</t>
+  </si>
+  <si>
+    <t>ED (3,2,2)</t>
   </si>
 </sst>
 </file>
@@ -643,13 +646,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2695,7 +2698,7 @@
   <dimension ref="A1:M100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H4:M14"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2732,7 +2735,7 @@
         <v>7</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>3</v>
@@ -2767,7 +2770,7 @@
         <v>12</v>
       </c>
       <c r="F2" s="16">
-        <f>SQRT(((A2-$H$2)^2)+((B2-$I$2)^2)+((C2-$J$2)^2))</f>
+        <f t="shared" ref="F2:F33" si="0">SQRT(((A2-$H$2)^2)+((B2-$I$2)^2)+((C2-$J$2)^2))</f>
         <v>0</v>
       </c>
       <c r="H2" s="3">
@@ -2801,7 +2804,7 @@
         <v>12</v>
       </c>
       <c r="F3" s="16">
-        <f>SQRT(((A3-$H$2)^2)+((B3-$I$2)^2)+((C3-$J$2)^2))</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2822,7 +2825,7 @@
         <v>12</v>
       </c>
       <c r="F4" s="16">
-        <f>SQRT(((A4-$H$2)^2)+((B4-$I$2)^2)+((C4-$J$2)^2))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H4" s="9" t="s">
@@ -2846,7 +2849,7 @@
         <v>9</v>
       </c>
       <c r="F5" s="16">
-        <f>SQRT(((A5-$H$2)^2)+((B5-$I$2)^2)+((C5-$J$2)^2))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H5" s="2" t="s">
@@ -2885,7 +2888,7 @@
         <v>12</v>
       </c>
       <c r="F6" s="16">
-        <f>SQRT(((A6-$H$2)^2)+((B6-$I$2)^2)+((C6-$J$2)^2))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H6" s="3">
@@ -2925,7 +2928,7 @@
         <v>10</v>
       </c>
       <c r="F7" s="16">
-        <f>SQRT(((A7-$H$2)^2)+((B7-$I$2)^2)+((C7-$J$2)^2))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H7" s="3">
@@ -2965,7 +2968,7 @@
         <v>12</v>
       </c>
       <c r="F8" s="16">
-        <f>SQRT(((A8-$H$2)^2)+((B8-$I$2)^2)+((C8-$J$2)^2))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H8" s="3">
@@ -3005,7 +3008,7 @@
         <v>9</v>
       </c>
       <c r="F9" s="16">
-        <f>SQRT(((A9-$H$2)^2)+((B9-$I$2)^2)+((C9-$J$2)^2))</f>
+        <f t="shared" si="0"/>
         <v>1.4142135623730951</v>
       </c>
       <c r="H9" s="3">
@@ -3045,7 +3048,7 @@
         <v>9</v>
       </c>
       <c r="F10" s="16">
-        <f>SQRT(((A10-$H$2)^2)+((B10-$I$2)^2)+((C10-$J$2)^2))</f>
+        <f t="shared" si="0"/>
         <v>1.4142135623730951</v>
       </c>
       <c r="H10" s="3">
@@ -3085,7 +3088,7 @@
         <v>9</v>
       </c>
       <c r="F11" s="16">
-        <f>SQRT(((A11-$H$2)^2)+((B11-$I$2)^2)+((C11-$J$2)^2))</f>
+        <f t="shared" si="0"/>
         <v>1.4142135623730951</v>
       </c>
     </row>
@@ -3106,7 +3109,7 @@
         <v>9</v>
       </c>
       <c r="F12" s="16">
-        <f>SQRT(((A12-$H$2)^2)+((B12-$I$2)^2)+((C12-$J$2)^2))</f>
+        <f t="shared" si="0"/>
         <v>1.4142135623730951</v>
       </c>
       <c r="H12" s="7" t="s">
@@ -3134,7 +3137,7 @@
         <v>9</v>
       </c>
       <c r="F13" s="16">
-        <f>SQRT(((A13-$H$2)^2)+((B13-$I$2)^2)+((C13-$J$2)^2))</f>
+        <f t="shared" si="0"/>
         <v>1.4142135623730951</v>
       </c>
       <c r="H13" s="7" t="s">
@@ -3162,7 +3165,7 @@
         <v>9</v>
       </c>
       <c r="F14" s="16">
-        <f>SQRT(((A14-$H$2)^2)+((B14-$I$2)^2)+((C14-$J$2)^2))</f>
+        <f t="shared" si="0"/>
         <v>1.4142135623730951</v>
       </c>
       <c r="H14" s="7" t="s">
@@ -3190,7 +3193,7 @@
         <v>9</v>
       </c>
       <c r="F15" s="16">
-        <f>SQRT(((A15-$H$2)^2)+((B15-$I$2)^2)+((C15-$J$2)^2))</f>
+        <f t="shared" si="0"/>
         <v>1.4142135623730951</v>
       </c>
     </row>
@@ -3211,7 +3214,7 @@
         <v>9</v>
       </c>
       <c r="F16" s="16">
-        <f>SQRT(((A16-$H$2)^2)+((B16-$I$2)^2)+((C16-$J$2)^2))</f>
+        <f t="shared" si="0"/>
         <v>1.7320508075688772</v>
       </c>
     </row>
@@ -3232,7 +3235,7 @@
         <v>9</v>
       </c>
       <c r="F17" s="16">
-        <f>SQRT(((A17-$H$2)^2)+((B17-$I$2)^2)+((C17-$J$2)^2))</f>
+        <f t="shared" si="0"/>
         <v>1.7320508075688772</v>
       </c>
     </row>
@@ -3253,7 +3256,7 @@
         <v>9</v>
       </c>
       <c r="F18" s="16">
-        <f>SQRT(((A18-$H$2)^2)+((B18-$I$2)^2)+((C18-$J$2)^2))</f>
+        <f t="shared" si="0"/>
         <v>1.7320508075688772</v>
       </c>
     </row>
@@ -3274,7 +3277,7 @@
         <v>9</v>
       </c>
       <c r="F19" s="16">
-        <f>SQRT(((A19-$H$2)^2)+((B19-$I$2)^2)+((C19-$J$2)^2))</f>
+        <f t="shared" si="0"/>
         <v>1.7320508075688772</v>
       </c>
     </row>
@@ -3295,7 +3298,7 @@
         <v>12</v>
       </c>
       <c r="F20" s="16">
-        <f>SQRT(((A20-$H$2)^2)+((B20-$I$2)^2)+((C20-$J$2)^2))</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -3316,7 +3319,7 @@
         <v>12</v>
       </c>
       <c r="F21" s="16">
-        <f>SQRT(((A21-$H$2)^2)+((B21-$I$2)^2)+((C21-$J$2)^2))</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -3337,7 +3340,7 @@
         <v>9</v>
       </c>
       <c r="F22" s="16">
-        <f>SQRT(((A22-$H$2)^2)+((B22-$I$2)^2)+((C22-$J$2)^2))</f>
+        <f t="shared" si="0"/>
         <v>2.2360679774997898</v>
       </c>
     </row>
@@ -3358,7 +3361,7 @@
         <v>9</v>
       </c>
       <c r="F23" s="16">
-        <f>SQRT(((A23-$H$2)^2)+((B23-$I$2)^2)+((C23-$J$2)^2))</f>
+        <f t="shared" si="0"/>
         <v>2.2360679774997898</v>
       </c>
     </row>
@@ -3379,7 +3382,7 @@
         <v>9</v>
       </c>
       <c r="F24" s="16">
-        <f>SQRT(((A24-$H$2)^2)+((B24-$I$2)^2)+((C24-$J$2)^2))</f>
+        <f t="shared" si="0"/>
         <v>2.2360679774997898</v>
       </c>
     </row>
@@ -3400,7 +3403,7 @@
         <v>12</v>
       </c>
       <c r="F25" s="16">
-        <f>SQRT(((A25-$H$2)^2)+((B25-$I$2)^2)+((C25-$J$2)^2))</f>
+        <f t="shared" si="0"/>
         <v>2.2360679774997898</v>
       </c>
     </row>
@@ -3421,7 +3424,7 @@
         <v>12</v>
       </c>
       <c r="F26" s="16">
-        <f>SQRT(((A26-$H$2)^2)+((B26-$I$2)^2)+((C26-$J$2)^2))</f>
+        <f t="shared" si="0"/>
         <v>2.2360679774997898</v>
       </c>
     </row>
@@ -3442,7 +3445,7 @@
         <v>12</v>
       </c>
       <c r="F27" s="16">
-        <f>SQRT(((A27-$H$2)^2)+((B27-$I$2)^2)+((C27-$J$2)^2))</f>
+        <f t="shared" si="0"/>
         <v>2.2360679774997898</v>
       </c>
     </row>
@@ -3463,7 +3466,7 @@
         <v>9</v>
       </c>
       <c r="F28" s="16">
-        <f>SQRT(((A28-$H$2)^2)+((B28-$I$2)^2)+((C28-$J$2)^2))</f>
+        <f t="shared" si="0"/>
         <v>2.2360679774997898</v>
       </c>
     </row>
@@ -3484,7 +3487,7 @@
         <v>9</v>
       </c>
       <c r="F29" s="16">
-        <f>SQRT(((A29-$H$2)^2)+((B29-$I$2)^2)+((C29-$J$2)^2))</f>
+        <f t="shared" si="0"/>
         <v>2.2360679774997898</v>
       </c>
     </row>
@@ -3505,7 +3508,7 @@
         <v>12</v>
       </c>
       <c r="F30" s="16">
-        <f>SQRT(((A30-$H$2)^2)+((B30-$I$2)^2)+((C30-$J$2)^2))</f>
+        <f t="shared" si="0"/>
         <v>2.2360679774997898</v>
       </c>
     </row>
@@ -3526,7 +3529,7 @@
         <v>12</v>
       </c>
       <c r="F31" s="16">
-        <f>SQRT(((A31-$H$2)^2)+((B31-$I$2)^2)+((C31-$J$2)^2))</f>
+        <f t="shared" si="0"/>
         <v>2.2360679774997898</v>
       </c>
     </row>
@@ -3547,7 +3550,7 @@
         <v>9</v>
       </c>
       <c r="F32" s="16">
-        <f>SQRT(((A32-$H$2)^2)+((B32-$I$2)^2)+((C32-$J$2)^2))</f>
+        <f t="shared" si="0"/>
         <v>2.4494897427831779</v>
       </c>
     </row>
@@ -3568,7 +3571,7 @@
         <v>12</v>
       </c>
       <c r="F33" s="16">
-        <f>SQRT(((A33-$H$2)^2)+((B33-$I$2)^2)+((C33-$J$2)^2))</f>
+        <f t="shared" si="0"/>
         <v>2.4494897427831779</v>
       </c>
     </row>
@@ -3589,7 +3592,7 @@
         <v>9</v>
       </c>
       <c r="F34" s="16">
-        <f>SQRT(((A34-$H$2)^2)+((B34-$I$2)^2)+((C34-$J$2)^2))</f>
+        <f t="shared" ref="F34:F62" si="1">SQRT(((A34-$H$2)^2)+((B34-$I$2)^2)+((C34-$J$2)^2))</f>
         <v>2.4494897427831779</v>
       </c>
     </row>
@@ -3610,7 +3613,7 @@
         <v>10</v>
       </c>
       <c r="F35" s="16">
-        <f>SQRT(((A35-$H$2)^2)+((B35-$I$2)^2)+((C35-$J$2)^2))</f>
+        <f t="shared" si="1"/>
         <v>2.8284271247461903</v>
       </c>
     </row>
@@ -3631,7 +3634,7 @@
         <v>9</v>
       </c>
       <c r="F36" s="16">
-        <f>SQRT(((A36-$H$2)^2)+((B36-$I$2)^2)+((C36-$J$2)^2))</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
     </row>
@@ -3652,7 +3655,7 @@
         <v>9</v>
       </c>
       <c r="F37" s="16">
-        <f>SQRT(((A37-$H$2)^2)+((B37-$I$2)^2)+((C37-$J$2)^2))</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
     </row>
@@ -3673,7 +3676,7 @@
         <v>9</v>
       </c>
       <c r="F38" s="16">
-        <f>SQRT(((A38-$H$2)^2)+((B38-$I$2)^2)+((C38-$J$2)^2))</f>
+        <f t="shared" si="1"/>
         <v>3.1622776601683795</v>
       </c>
     </row>
@@ -3694,7 +3697,7 @@
         <v>9</v>
       </c>
       <c r="F39" s="16">
-        <f>SQRT(((A39-$H$2)^2)+((B39-$I$2)^2)+((C39-$J$2)^2))</f>
+        <f t="shared" si="1"/>
         <v>3.1622776601683795</v>
       </c>
     </row>
@@ -3715,7 +3718,7 @@
         <v>12</v>
       </c>
       <c r="F40" s="16">
-        <f>SQRT(((A40-$H$2)^2)+((B40-$I$2)^2)+((C40-$J$2)^2))</f>
+        <f t="shared" si="1"/>
         <v>3.1622776601683795</v>
       </c>
     </row>
@@ -3736,7 +3739,7 @@
         <v>12</v>
       </c>
       <c r="F41" s="16">
-        <f>SQRT(((A41-$H$2)^2)+((B41-$I$2)^2)+((C41-$J$2)^2))</f>
+        <f t="shared" si="1"/>
         <v>3.1622776601683795</v>
       </c>
     </row>
@@ -3757,7 +3760,7 @@
         <v>9</v>
       </c>
       <c r="F42" s="16">
-        <f>SQRT(((A42-$H$2)^2)+((B42-$I$2)^2)+((C42-$J$2)^2))</f>
+        <f t="shared" si="1"/>
         <v>3.3166247903553998</v>
       </c>
     </row>
@@ -3778,7 +3781,7 @@
         <v>9</v>
       </c>
       <c r="F43" s="16">
-        <f>SQRT(((A43-$H$2)^2)+((B43-$I$2)^2)+((C43-$J$2)^2))</f>
+        <f t="shared" si="1"/>
         <v>3.3166247903553998</v>
       </c>
     </row>
@@ -3799,7 +3802,7 @@
         <v>10</v>
       </c>
       <c r="F44" s="16">
-        <f>SQRT(((A44-$H$2)^2)+((B44-$I$2)^2)+((C44-$J$2)^2))</f>
+        <f t="shared" si="1"/>
         <v>3.6055512754639891</v>
       </c>
     </row>
@@ -3820,7 +3823,7 @@
         <v>9</v>
       </c>
       <c r="F45" s="16">
-        <f>SQRT(((A45-$H$2)^2)+((B45-$I$2)^2)+((C45-$J$2)^2))</f>
+        <f t="shared" si="1"/>
         <v>3.7416573867739413</v>
       </c>
     </row>
@@ -3841,7 +3844,7 @@
         <v>12</v>
       </c>
       <c r="F46" s="16">
-        <f>SQRT(((A46-$H$2)^2)+((B46-$I$2)^2)+((C46-$J$2)^2))</f>
+        <f t="shared" si="1"/>
         <v>3.7416573867739413</v>
       </c>
     </row>
@@ -3862,7 +3865,7 @@
         <v>9</v>
       </c>
       <c r="F47" s="16">
-        <f>SQRT(((A47-$H$2)^2)+((B47-$I$2)^2)+((C47-$J$2)^2))</f>
+        <f t="shared" si="1"/>
         <v>4.1231056256176606</v>
       </c>
     </row>
@@ -3883,7 +3886,7 @@
         <v>12</v>
       </c>
       <c r="F48" s="16">
-        <f>SQRT(((A48-$H$2)^2)+((B48-$I$2)^2)+((C48-$J$2)^2))</f>
+        <f t="shared" si="1"/>
         <v>4.1231056256176606</v>
       </c>
     </row>
@@ -3904,7 +3907,7 @@
         <v>12</v>
       </c>
       <c r="F49" s="16">
-        <f>SQRT(((A49-$H$2)^2)+((B49-$I$2)^2)+((C49-$J$2)^2))</f>
+        <f t="shared" si="1"/>
         <v>4.1231056256176606</v>
       </c>
     </row>
@@ -3925,7 +3928,7 @@
         <v>10</v>
       </c>
       <c r="F50" s="16">
-        <f>SQRT(((A50-$H$2)^2)+((B50-$I$2)^2)+((C50-$J$2)^2))</f>
+        <f t="shared" si="1"/>
         <v>4.1231056256176606</v>
       </c>
     </row>
@@ -3946,7 +3949,7 @@
         <v>9</v>
       </c>
       <c r="F51" s="16">
-        <f>SQRT(((A51-$H$2)^2)+((B51-$I$2)^2)+((C51-$J$2)^2))</f>
+        <f t="shared" si="1"/>
         <v>4.2426406871192848</v>
       </c>
     </row>
@@ -3967,7 +3970,7 @@
         <v>12</v>
       </c>
       <c r="F52" s="16">
-        <f>SQRT(((A52-$H$2)^2)+((B52-$I$2)^2)+((C52-$J$2)^2))</f>
+        <f t="shared" si="1"/>
         <v>4.4721359549995796</v>
       </c>
     </row>
@@ -3988,7 +3991,7 @@
         <v>12</v>
       </c>
       <c r="F53" s="16">
-        <f>SQRT(((A53-$H$2)^2)+((B53-$I$2)^2)+((C53-$J$2)^2))</f>
+        <f t="shared" si="1"/>
         <v>4.5825756949558398</v>
       </c>
     </row>
@@ -4009,7 +4012,7 @@
         <v>9</v>
       </c>
       <c r="F54" s="16">
-        <f>SQRT(((A54-$H$2)^2)+((B54-$I$2)^2)+((C54-$J$2)^2))</f>
+        <f t="shared" si="1"/>
         <v>4.5825756949558398</v>
       </c>
     </row>
@@ -4030,7 +4033,7 @@
         <v>10</v>
       </c>
       <c r="F55" s="16">
-        <f>SQRT(((A55-$H$2)^2)+((B55-$I$2)^2)+((C55-$J$2)^2))</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
     </row>
@@ -4051,7 +4054,7 @@
         <v>12</v>
       </c>
       <c r="F56" s="16">
-        <f>SQRT(((A56-$H$2)^2)+((B56-$I$2)^2)+((C56-$J$2)^2))</f>
+        <f t="shared" si="1"/>
         <v>5.0990195135927845</v>
       </c>
     </row>
@@ -4072,7 +4075,7 @@
         <v>12</v>
       </c>
       <c r="F57" s="16">
-        <f>SQRT(((A57-$H$2)^2)+((B57-$I$2)^2)+((C57-$J$2)^2))</f>
+        <f t="shared" si="1"/>
         <v>5.0990195135927845</v>
       </c>
     </row>
@@ -4093,7 +4096,7 @@
         <v>12</v>
       </c>
       <c r="F58" s="16">
-        <f>SQRT(((A58-$H$2)^2)+((B58-$I$2)^2)+((C58-$J$2)^2))</f>
+        <f t="shared" si="1"/>
         <v>5.0990195135927845</v>
       </c>
     </row>
@@ -4114,7 +4117,7 @@
         <v>9</v>
       </c>
       <c r="F59" s="16">
-        <f>SQRT(((A59-$H$2)^2)+((B59-$I$2)^2)+((C59-$J$2)^2))</f>
+        <f t="shared" si="1"/>
         <v>5.196152422706632</v>
       </c>
     </row>
@@ -4135,7 +4138,7 @@
         <v>9</v>
       </c>
       <c r="F60" s="16">
-        <f>SQRT(((A60-$H$2)^2)+((B60-$I$2)^2)+((C60-$J$2)^2))</f>
+        <f t="shared" si="1"/>
         <v>5.196152422706632</v>
       </c>
     </row>
@@ -4156,7 +4159,7 @@
         <v>12</v>
       </c>
       <c r="F61" s="16">
-        <f>SQRT(((A61-$H$2)^2)+((B61-$I$2)^2)+((C61-$J$2)^2))</f>
+        <f t="shared" si="1"/>
         <v>5.3851648071345037</v>
       </c>
     </row>
@@ -4177,7 +4180,7 @@
         <v>9</v>
       </c>
       <c r="F62" s="16">
-        <f>SQRT(((A62-$H$2)^2)+((B62-$I$2)^2)+((C62-$J$2)^2))</f>
+        <f t="shared" si="1"/>
         <v>5.4772255750516612</v>
       </c>
     </row>
@@ -4230,7 +4233,7 @@
         <v>9</v>
       </c>
       <c r="F67" s="15">
-        <f t="shared" ref="F67:F68" si="0">SQRT(((A67-$H$2)^2)+((B67-$I$2)^2)+((C67-$J$2)^2))</f>
+        <f t="shared" ref="F67:F68" si="2">SQRT(((A67-$H$2)^2)+((B67-$I$2)^2)+((C67-$J$2)^2))</f>
         <v>4.5825756949558398</v>
       </c>
     </row>
@@ -4251,7 +4254,7 @@
         <v>9</v>
       </c>
       <c r="F68" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>5.4772255750516612</v>
       </c>
     </row>
@@ -7909,6 +7912,18 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="I22:I23"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="H22:H23"/>
+    <mergeCell ref="G12:I12"/>
+    <mergeCell ref="K12:M12"/>
+    <mergeCell ref="K13:K14"/>
+    <mergeCell ref="L13:L14"/>
+    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="I13:I14"/>
     <mergeCell ref="A1:P2"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="A5:A6"/>
@@ -7924,18 +7939,6 @@
     <mergeCell ref="L5:L6"/>
     <mergeCell ref="G5:G6"/>
     <mergeCell ref="H5:H6"/>
-    <mergeCell ref="K12:M12"/>
-    <mergeCell ref="K13:K14"/>
-    <mergeCell ref="L13:L14"/>
-    <mergeCell ref="M13:M14"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="I22:I23"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="H22:H23"/>
-    <mergeCell ref="G12:I12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
@@ -7997,7 +8000,7 @@
       <c r="G2" s="44" t="s">
         <v>84</v>
       </c>
-      <c r="H2" s="45" t="s">
+      <c r="H2" s="47" t="s">
         <v>43</v>
       </c>
       <c r="I2" s="42" t="s">
@@ -8130,7 +8133,7 @@
         <f t="shared" si="1"/>
         <v>Naik</v>
       </c>
-      <c r="H7" s="47" t="s">
+      <c r="H7" s="46" t="s">
         <v>41</v>
       </c>
       <c r="I7" s="44" t="s">
@@ -8473,7 +8476,7 @@
         <f t="shared" si="1"/>
         <v>Naik</v>
       </c>
-      <c r="H15" s="46" t="s">
+      <c r="H15" s="45" t="s">
         <v>84</v>
       </c>
       <c r="I15" s="34"/>
@@ -8747,6 +8750,16 @@
     <row r="100" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
     <mergeCell ref="N7:N8"/>
     <mergeCell ref="H15:I15"/>
     <mergeCell ref="H7:H8"/>
@@ -8755,16 +8768,6 @@
     <mergeCell ref="K7:K8"/>
     <mergeCell ref="L7:L8"/>
     <mergeCell ref="M7:M8"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="H2:H3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>